<commit_message>
update README. Add options table.
</commit_message>
<xml_diff>
--- a/tables/options.xlsx
+++ b/tables/options.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -120,28 +120,43 @@
     <t>If true then direction the transformTarget tilts is reversed. If you want to affect only one axis then use `tiltXReverse` or `tiltYReverse`.</t>
   </si>
   <si>
-    <t>Sets which DOM Element the event listener will be created on the detect the mouse position for the animation. If not defined then sets the transformTarget to be the hoverTarget as well.</t>
-  </si>
-  <si>
     <t>Number (1|2|3)</t>
   </si>
   <si>
     <t>Accepts either 1, 2, or 3. Sets a different way the rotatation is calculated depending on mouse position. Please see example for details.</t>
   </si>
   <si>
-    <t>When hovering over hoverTarget then scales to this value.</t>
-  </si>
-  <si>
     <t>Sets initial transform properties in case your element already has some transform properties on it or you want it to start at a different position.</t>
   </si>
   <si>
     <t>Specifies the speed curve of the transition effect. Default is "cubic-bezier(0.215, 0.61, 0.355, 1)".</t>
   </si>
   <si>
-    <t>If true then when mouse leaves hoverTarget then it resets position of transformTarget.</t>
-  </si>
-  <si>
     <t>How many milliseconds/seconds it takes for a transform transition to complete.</t>
+  </si>
+  <si>
+    <t>enterCB</t>
+  </si>
+  <si>
+    <t>leaveCB</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Callback function that fires when mouse leaves hoverTarget.</t>
+  </si>
+  <si>
+    <t>Callback function that fires when mouse enters hoverTarget.</t>
+  </si>
+  <si>
+    <t>Sets which DOM Element the event listener will be created on the detect the mouse position for the animation. If not defined then sets the `transformTarget` to be the `hoverTarget` as well.</t>
+  </si>
+  <si>
+    <t>Hovering over hoverTarget scales to this value.</t>
+  </si>
+  <si>
+    <t>If true, then when mouse leaves hoverTarget then it resets position of transformTarget.</t>
   </si>
 </sst>
 </file>
@@ -480,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +533,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -624,13 +639,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -644,7 +659,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -658,7 +673,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -672,7 +687,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -686,7 +701,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -700,11 +715,40 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix resetPosition with tilt bug. Add codePen link to excel for hoverTarget.
</commit_message>
<xml_diff>
--- a/tables/options.xlsx
+++ b/tables/options.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="24240" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>If true, then when mouse leaves hoverTarget then it resets position of transformTarget.</t>
+  </si>
+  <si>
+    <t>[CodePen](https://codepen.io/maiCoding/pen/XoaQKG)</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +533,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
update todo and excel sheet
</commit_message>
<xml_diff>
--- a/tables/options.xlsx
+++ b/tables/options.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="24240" windowHeight="12600"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Number (degrees)</t>
   </si>
   <si>
-    <t>Number (ratio)</t>
-  </si>
-  <si>
     <t>Object</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>If true then direction the transformTarget tilts is reversed. If you want to affect only one axis then use `tiltXReverse` or `tiltYReverse`.</t>
   </si>
   <si>
-    <t>Number (1|2|3)</t>
-  </si>
-  <si>
     <t>Accepts either 1, 2, or 3. Sets a different way the rotatation is calculated depending on mouse position. Please see example for details.</t>
   </si>
   <si>
@@ -132,9 +126,6 @@
     <t>Specifies the speed curve of the transition effect. Default is "cubic-bezier(0.215, 0.61, 0.355, 1)".</t>
   </si>
   <si>
-    <t>How many milliseconds/seconds it takes for a transform transition to complete.</t>
-  </si>
-  <si>
     <t>enterCB</t>
   </si>
   <si>
@@ -153,13 +144,34 @@
     <t>Sets which DOM Element the event listener will be created on the detect the mouse position for the animation. If not defined then sets the `transformTarget` to be the `hoverTarget` as well.</t>
   </si>
   <si>
-    <t>Hovering over hoverTarget scales to this value.</t>
-  </si>
-  <si>
     <t>If true, then when mouse leaves hoverTarget then it resets position of transformTarget.</t>
   </si>
   <si>
     <t>[CodePen](https://codepen.io/maiCoding/pen/XoaQKG)</t>
+  </si>
+  <si>
+    <t>Number (milliseconds) \| String</t>
+  </si>
+  <si>
+    <t>Number (1\|2\|3)</t>
+  </si>
+  <si>
+    <t>Number (float)</t>
+  </si>
+  <si>
+    <t>Hovering over hoverTarget scales to this value. 1 = 100%</t>
+  </si>
+  <si>
+    <t>[CodePen](https://codepen.io/maiCoding/pen/MZEMqv)</t>
+  </si>
+  <si>
+    <t>[CodePen](https://codepen.io/maiCoding/pen/ZVaLOp)</t>
+  </si>
+  <si>
+    <t>[CodePen](https://codepen.io/maiCoding/pen/aPVQmw)</t>
+  </si>
+  <si>
+    <t>How many milliseconds/seconds it takes for a transform transition to complete. Default is 200ms</t>
   </si>
 </sst>
 </file>
@@ -501,7 +513,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,10 +545,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -547,10 +559,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -561,10 +573,10 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -575,10 +587,10 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -589,10 +601,10 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -603,10 +615,10 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -620,7 +632,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -634,7 +646,7 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -642,13 +654,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -656,13 +668,13 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -670,27 +682,27 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -698,13 +710,13 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -718,35 +730,35 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add onChange. change callback variables names
</commit_message>
<xml_diff>
--- a/tables/options.xlsx
+++ b/tables/options.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -126,12 +126,6 @@
     <t>Specifies the speed curve of the transition effect. Default is "cubic-bezier(0.215, 0.61, 0.355, 1)".</t>
   </si>
   <si>
-    <t>enterCB</t>
-  </si>
-  <si>
-    <t>leaveCB</t>
-  </si>
-  <si>
     <t>Function</t>
   </si>
   <si>
@@ -172,6 +166,18 @@
   </si>
   <si>
     <t>How many milliseconds/seconds it takes for a transform transition to complete. Default is 200ms</t>
+  </si>
+  <si>
+    <t>onEnter</t>
+  </si>
+  <si>
+    <t>onLeave</t>
+  </si>
+  <si>
+    <t>onChange</t>
+  </si>
+  <si>
+    <t>Callback function that fires when mouse moves inside of hoverTarget and a new transition is fired.</t>
   </si>
 </sst>
 </file>
@@ -510,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,10 +551,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -559,7 +565,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -573,7 +579,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
@@ -587,7 +593,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -601,7 +607,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
@@ -615,7 +621,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -654,7 +660,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -668,13 +674,13 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -696,13 +702,13 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,35 +736,49 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
         <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>39</v>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add onChange. change callback variables names (#6)
</commit_message>
<xml_diff>
--- a/tables/options.xlsx
+++ b/tables/options.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -126,12 +126,6 @@
     <t>Specifies the speed curve of the transition effect. Default is "cubic-bezier(0.215, 0.61, 0.355, 1)".</t>
   </si>
   <si>
-    <t>enterCB</t>
-  </si>
-  <si>
-    <t>leaveCB</t>
-  </si>
-  <si>
     <t>Function</t>
   </si>
   <si>
@@ -172,6 +166,18 @@
   </si>
   <si>
     <t>How many milliseconds/seconds it takes for a transform transition to complete. Default is 200ms</t>
+  </si>
+  <si>
+    <t>onEnter</t>
+  </si>
+  <si>
+    <t>onLeave</t>
+  </si>
+  <si>
+    <t>onChange</t>
+  </si>
+  <si>
+    <t>Callback function that fires when mouse moves inside of hoverTarget and a new transition is fired.</t>
   </si>
 </sst>
 </file>
@@ -510,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,10 +551,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -559,7 +565,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -573,7 +579,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
@@ -587,7 +593,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -601,7 +607,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
@@ -615,7 +621,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -654,7 +660,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -668,13 +674,13 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -696,13 +702,13 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,35 +736,49 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
         <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>39</v>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "add onChange. change callback variables names (#6)"
This reverts commit 65e301555543c0d227d66c4b829f1923d06e2171.
</commit_message>
<xml_diff>
--- a/tables/options.xlsx
+++ b/tables/options.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -126,6 +126,12 @@
     <t>Specifies the speed curve of the transition effect. Default is "cubic-bezier(0.215, 0.61, 0.355, 1)".</t>
   </si>
   <si>
+    <t>enterCB</t>
+  </si>
+  <si>
+    <t>leaveCB</t>
+  </si>
+  <si>
     <t>Function</t>
   </si>
   <si>
@@ -166,18 +172,6 @@
   </si>
   <si>
     <t>How many milliseconds/seconds it takes for a transform transition to complete. Default is 200ms</t>
-  </si>
-  <si>
-    <t>onEnter</t>
-  </si>
-  <si>
-    <t>onLeave</t>
-  </si>
-  <si>
-    <t>onChange</t>
-  </si>
-  <si>
-    <t>Callback function that fires when mouse moves inside of hoverTarget and a new transition is fired.</t>
   </si>
 </sst>
 </file>
@@ -516,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,10 +545,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -565,7 +559,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -579,7 +573,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
@@ -593,7 +587,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -607,7 +601,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
@@ -621,7 +615,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -660,7 +654,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -674,13 +668,13 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,13 +696,13 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -736,49 +730,35 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "add onChange. change callback variables names (#6)" (#7)
This reverts commit 65e301555543c0d227d66c4b829f1923d06e2171.
</commit_message>
<xml_diff>
--- a/tables/options.xlsx
+++ b/tables/options.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -126,6 +126,12 @@
     <t>Specifies the speed curve of the transition effect. Default is "cubic-bezier(0.215, 0.61, 0.355, 1)".</t>
   </si>
   <si>
+    <t>enterCB</t>
+  </si>
+  <si>
+    <t>leaveCB</t>
+  </si>
+  <si>
     <t>Function</t>
   </si>
   <si>
@@ -166,18 +172,6 @@
   </si>
   <si>
     <t>How many milliseconds/seconds it takes for a transform transition to complete. Default is 200ms</t>
-  </si>
-  <si>
-    <t>onEnter</t>
-  </si>
-  <si>
-    <t>onLeave</t>
-  </si>
-  <si>
-    <t>onChange</t>
-  </si>
-  <si>
-    <t>Callback function that fires when mouse moves inside of hoverTarget and a new transition is fired.</t>
   </si>
 </sst>
 </file>
@@ -516,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,10 +545,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -565,7 +559,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -579,7 +573,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
@@ -593,7 +587,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -607,7 +601,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
@@ -621,7 +615,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -660,7 +654,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -674,13 +668,13 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,13 +696,13 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -736,49 +730,35 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>